<commit_message>
Features Added: Sending an Email Reading Excel Config File Code Divided in Multiple Files Restructuring Main Sequence into Flowchart
</commit_message>
<xml_diff>
--- a/Bucuresti Nord-Constanta.xlsx
+++ b/Bucuresti Nord-Constanta.xlsx
@@ -8,17 +8,63 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Test</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+  <si>
+    <t>Train Information</t>
+  </si>
+  <si>
+    <t>From:</t>
+  </si>
+  <si>
+    <t>Bucuresti Nord</t>
+  </si>
+  <si>
+    <t>To:</t>
+  </si>
+  <si>
+    <t>Constanta</t>
+  </si>
+  <si>
+    <t>Departure Time</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>Arrival Time</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>+19 min întârziere</t>
+  </si>
+  <si>
+    <t>la timp</t>
+  </si>
+  <si>
+    <t>-1 min mai devreme</t>
+  </si>
+  <si>
+    <t>+4 min întârziere</t>
+  </si>
+  <si>
+    <t>+2 min întârziere</t>
+  </si>
+  <si>
+    <t>+20 min întârziere</t>
+  </si>
+  <si>
+    <t>sosește cu 102 min întârziere la Constanța*</t>
+  </si>
+  <si>
+    <t>sosește la timp la Constanța*</t>
   </si>
 </sst>
 </file>
@@ -54,8 +100,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,42 +404,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.47291666666666665</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.39513888888888887</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.44930555555555557</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.48402777777777778</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.5395833333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.58750000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.62916666666666665</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.70138888888888884</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0.64027777777777783</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.74861111111111101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.68958333333333333</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.79236111111111107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.81736111111111109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.87916666666666676</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0.8520833333333333</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.95833333333333337</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Edit: Code either runs continuously or one time (set in config) New: When code runs continuously, it waits for emails to enter inbox, then replies to the requests in them.
</commit_message>
<xml_diff>
--- a/Bucuresti Nord-Constanta.xlsx
+++ b/Bucuresti Nord-Constanta.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Train Information</t>
   </si>
@@ -43,28 +43,22 @@
     <t>Length</t>
   </si>
   <si>
-    <t>+19 min întârziere</t>
+    <t>+6 min întârziere</t>
+  </si>
+  <si>
+    <t>+3 min întârziere</t>
   </si>
   <si>
     <t>la timp</t>
   </si>
   <si>
-    <t>-1 min mai devreme</t>
-  </si>
-  <si>
-    <t>+4 min întârziere</t>
-  </si>
-  <si>
-    <t>+2 min întârziere</t>
-  </si>
-  <si>
-    <t>+20 min întârziere</t>
-  </si>
-  <si>
-    <t>sosește cu 102 min întârziere la Constanța*</t>
+    <t>sosește cu 35 min întârziere la Constanța*</t>
   </si>
   <si>
     <t>sosește la timp la Constanța*</t>
+  </si>
+  <si>
+    <t>pleacă la timp din București Nord*</t>
   </si>
 </sst>
 </file>
@@ -468,7 +462,7 @@
         <v>0.34722222222222227</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
         <v>0.44930555555555557</v>
@@ -490,7 +484,7 @@
         <v>0.4375</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1">
         <v>0.5395833333333333</v>
@@ -501,7 +495,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1">
         <v>0.58750000000000002</v>
@@ -512,7 +506,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1">
         <v>0.62916666666666665</v>
@@ -523,7 +517,7 @@
         <v>0.59722222222222221</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1">
         <v>0.70138888888888884</v>
@@ -534,7 +528,7 @@
         <v>0.64027777777777783</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>0.74861111111111101</v>
@@ -545,7 +539,7 @@
         <v>0.68958333333333333</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1">
         <v>0.79236111111111107</v>
@@ -556,7 +550,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1">
         <v>0.81736111111111109</v>
@@ -567,7 +561,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1">
         <v>0.87916666666666676</v>
@@ -578,7 +572,7 @@
         <v>0.8520833333333333</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
         <v>0.95833333333333337</v>

</xml_diff>